<commit_message>
edited protocol, ER diagram
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shark333\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Protokoll" sheetId="1" r:id="rId1"/>
+    <sheet name="Protocol" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -103,10 +103,13 @@
     <t>zusätzliche Recherche responsive WPF, Finalisierung des Datenmodells, Detaillierte Erhebung der Funktionen jeder einzelnen Schiene</t>
   </si>
   <si>
-    <t>Anpassung Datenmodell, Recherche Webtechnologien, Einpflegung des Datenmodells, Erstellen von Triggern etc. Aufsetzen einer Testumgebung</t>
-  </si>
-  <si>
     <t>Webservice - erste Implementierungen</t>
+  </si>
+  <si>
+    <t>Erstellen von Triggern etc. Aufsetzen einer Testumgebung, Einpflegung des Datenmodells</t>
+  </si>
+  <si>
+    <t>Anpassung Datenmodell, Recherche Webtechnologien</t>
   </si>
 </sst>
 </file>
@@ -660,19 +663,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5703125" style="2"/>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="19" t="s">
         <v>11</v>
@@ -695,7 +698,7 @@
       </c>
       <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -728,7 +731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -747,7 +750,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -766,7 +769,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -774,9 +777,11 @@
         <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -785,7 +790,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
@@ -793,9 +798,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="9"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -804,7 +811,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -821,7 +828,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
@@ -836,7 +843,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -844,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -855,7 +862,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
@@ -874,119 +881,119 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1242,7 +1249,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated protocol & description
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,6 +310,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,12 +352,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -666,359 +666,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="11">
         <v>0</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C8" s="11">
         <v>0.8</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Revert "updated protocol & description""
This reverts commit 8862de69a561167dc6427ac95fd2baaf1827143a, reversing
changes made to 7eabc0604a5d782f5b4b66cbeb4d52e958879322.
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,6 +310,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,12 +352,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -666,359 +666,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="11">
         <v>0</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C8" s="11">
         <v>0.8</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Revert "Revert "updated protocol & description"""
This reverts commit cddb21c6d93d63121c256fbddc20c4b1fc36850f.
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,12 +310,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,6 +346,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -666,359 +666,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
-    <col min="2" max="11" width="39.6640625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>0.8</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.8</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>1</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Revert "updated protocol & description"
This reverts commit 7eabc0604a5d782f5b4b66cbeb4d52e958879322.
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,12 +310,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,6 +346,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -666,359 +666,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
-    <col min="2" max="11" width="39.6640625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>0.8</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.8</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>1</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated mockups and protocol
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Erstellen eines Logos, Fertigstellung vorherigen Sprints</t>
   </si>
   <si>
-    <t>Fertigstellung GUI Mockups; Erstellung der WPF-GUI-Fenster; Start Implementierung</t>
-  </si>
-  <si>
     <t>Fertigstellung - Funktionsbeschreibung der einzelnen Komponenten; Beginn Erstellung GUI-Mockups für Desktopanwendung; Ziele für 2. Sprint</t>
   </si>
   <si>
@@ -131,12 +128,18 @@
   </si>
   <si>
     <t>Erstellen von Triggern; SQL Queries und Anforderungen für den Webservice</t>
+  </si>
+  <si>
+    <t>Fertigstellung GUI Mockups; Start Erstellung der GUI-Struktur in WPF</t>
+  </si>
+  <si>
+    <t>Fertigstellung GUI-Struktur in WPF; Start Implementierung der Business Logic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -317,10 +320,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,15 +367,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -681,375 +681,379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.6640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
+    <col min="2" max="11" width="39.6640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E6" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="E6" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="D8" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.95</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="D10" s="11">
         <v>0.1</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1095,7 +1099,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 E4">
+  <conditionalFormatting sqref="E4 C4">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1305,7 +1309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated gui and protocol
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -157,7 +157,7 @@
     <t>Lesen von XAML-Dokumentation bzgl. Containerstrukturen; gefehlt am 22.12.2018</t>
   </si>
   <si>
-    <t>Implementierung Dashboard + User</t>
+    <t>Implementierung aller GUIs</t>
   </si>
 </sst>
 </file>
@@ -388,44 +388,44 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -745,8 +745,8 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5:I5"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,26 +758,26 @@
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -799,14 +799,14 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="19" t="s">
         <v>40</v>
       </c>
     </row>
@@ -832,10 +832,10 @@
       <c r="G3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="23"/>
+      <c r="I3" s="25"/>
       <c r="J3" s="18" t="s">
         <v>43</v>
       </c>
@@ -863,11 +863,13 @@
       <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="26">
-        <v>1</v>
-      </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="9"/>
+      <c r="H4" s="22">
+        <v>1</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="9">
+        <v>0.3</v>
+      </c>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -919,8 +921,8 @@
       <c r="G6" s="9">
         <v>0.2</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
@@ -946,8 +948,8 @@
       <c r="G7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
@@ -973,8 +975,8 @@
       <c r="G8" s="9">
         <v>0.5</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
@@ -998,8 +1000,8 @@
         <v>34</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
@@ -1023,8 +1025,8 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
@@ -1149,6 +1151,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H10:I10"/>
@@ -1158,11 +1165,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="B8">
     <cfRule type="colorScale" priority="21">
@@ -1200,7 +1202,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 C4">
+  <conditionalFormatting sqref="C4 E4">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
addded protocol entry and new sprints
</commit_message>
<xml_diff>
--- a/doku/Protocol.xlsx
+++ b/doku/Protocol.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shark333\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0B06A0-C571-420A-99F1-A1AA2FE2A0F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -188,6 +189,30 @@
   </si>
   <si>
     <t>Phrases-Words-Kompatibilität</t>
+  </si>
+  <si>
+    <t>6.Sprint</t>
+  </si>
+  <si>
+    <t>19.02.2018 - 01.03.2018</t>
+  </si>
+  <si>
+    <t>02.03.2018 - 15.03.2018</t>
+  </si>
+  <si>
+    <t>16.03.2018 - 05.04.2018</t>
+  </si>
+  <si>
+    <t>06.04.2018 - 16.04.2018</t>
+  </si>
+  <si>
+    <t>7.Sprint</t>
+  </si>
+  <si>
+    <t>Präsentationsvorbereitung</t>
+  </si>
+  <si>
+    <t>Zieldefinition für die Web Applikation bis zum Zielende</t>
   </si>
 </sst>
 </file>
@@ -248,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -369,12 +394,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -404,9 +440,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -424,35 +457,51 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -769,44 +818,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K11" sqref="K11"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5703125" style="2"/>
+    <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
+    <col min="2" max="15" width="39.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="21" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="22"/>
-    </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="30"/>
+      <c r="L1" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="32"/>
+      <c r="N1" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -826,18 +883,30 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -853,24 +922,28 @@
       <c r="E3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="19"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -892,18 +965,22 @@
       <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="25">
-        <v>1</v>
-      </c>
-      <c r="I4" s="26"/>
+      <c r="H4" s="23">
+        <v>1</v>
+      </c>
+      <c r="I4" s="24"/>
       <c r="J4" s="9">
         <v>1</v>
       </c>
       <c r="K4" s="9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="9"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -916,26 +993,34 @@
       <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="20" t="s">
+      <c r="I5" s="28"/>
+      <c r="J5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="K5" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="35"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="31"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="8">
@@ -956,16 +1041,24 @@
       <c r="G6" s="9">
         <v>0.2</v>
       </c>
-      <c r="H6" s="25">
-        <v>1</v>
-      </c>
-      <c r="I6" s="26"/>
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+      <c r="I6" s="24"/>
       <c r="J6" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="34"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -975,31 +1068,35 @@
       <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="18" t="s">
+      <c r="I7" s="22"/>
+      <c r="J7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="L7" s="17"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="8">
@@ -1020,18 +1117,22 @@
       <c r="G8" s="9">
         <v>1</v>
       </c>
-      <c r="H8" s="25">
-        <v>1</v>
-      </c>
-      <c r="I8" s="26"/>
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+      <c r="I8" s="24"/>
       <c r="J8" s="9">
         <v>1</v>
       </c>
       <c r="K8" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="9"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1044,28 +1145,32 @@
       <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="L9" s="19"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="8">
@@ -1086,138 +1191,149 @@
       <c r="G10" s="9">
         <v>1</v>
       </c>
-      <c r="H10" s="25">
-        <v>1</v>
-      </c>
-      <c r="I10" s="26"/>
+      <c r="H10" s="23">
+        <v>1</v>
+      </c>
+      <c r="I10" s="24"/>
       <c r="J10" s="9">
         <v>1</v>
       </c>
       <c r="K10" s="9">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H10:I10"/>
@@ -1227,13 +1343,92 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4 E4">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:E6">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:E8">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:E10">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:G4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1245,7 +1440,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="F6:G6">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1257,7 +1452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="F8:G8">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1269,7 +1464,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 C4">
+  <conditionalFormatting sqref="F10:G10">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1281,7 +1488,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
+  <conditionalFormatting sqref="H6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1293,7 +1500,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:E8">
+  <conditionalFormatting sqref="H8">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1305,7 +1512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:E10">
+  <conditionalFormatting sqref="H10">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1317,7 +1524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:G4">
+  <conditionalFormatting sqref="J4:K4">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1329,7 +1536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:G6">
+  <conditionalFormatting sqref="J6:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1341,7 +1548,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:G8">
+  <conditionalFormatting sqref="J8:K8">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1353,7 +1560,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:G10">
+  <conditionalFormatting sqref="J10:K10">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1365,7 +1572,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="D4">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1377,7 +1584,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
+  <conditionalFormatting sqref="L4:M4">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1389,7 +1596,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="L6:M6">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1401,7 +1608,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="L8:M8">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1413,7 +1620,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:K4">
+  <conditionalFormatting sqref="L10:M10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1425,7 +1632,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:K6">
+  <conditionalFormatting sqref="N4:O4">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1437,7 +1644,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
+  <conditionalFormatting sqref="N6:O6">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1449,7 +1656,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
+  <conditionalFormatting sqref="N8:O8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1461,7 +1668,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
+  <conditionalFormatting sqref="N10:O10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1486,7 +1693,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>